<commit_message>
to string almost correct
</commit_message>
<xml_diff>
--- a/truth table.xlsx
+++ b/truth table.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\dev\rust\math-eval\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06F5A2E3-F4B2-487D-9B68-FEA1A09F30E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0E2772E-B360-4517-B56E-9AD4712FF108}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="345" yWindow="360" windowWidth="38700" windowHeight="15885" xr2:uid="{D11C0042-871A-40E6-9C8F-06A0F0CE9C5E}"/>
+    <workbookView xWindow="690" yWindow="705" windowWidth="38700" windowHeight="15885" xr2:uid="{D11C0042-871A-40E6-9C8F-06A0F0CE9C5E}"/>
   </bookViews>
   <sheets>
     <sheet name="List1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="42">
   <si>
     <t>prazen imenovalec</t>
   </si>
@@ -44,82 +44,124 @@
     <t>števec enočlenik</t>
   </si>
   <si>
-    <t>((-2-3)/(-4))-5</t>
-  </si>
-  <si>
-    <t>1-((-2-3)/(-4))-5</t>
-  </si>
-  <si>
-    <t>1-(-2-3)-5</t>
-  </si>
-  <si>
-    <t>((-2-3))-5</t>
-  </si>
-  <si>
-    <t>1-(-2)-5</t>
-  </si>
-  <si>
-    <t>(-2-3)/(-4)-5</t>
-  </si>
-  <si>
-    <t>1-((-2-3))-5</t>
-  </si>
-  <si>
-    <t>1-((-2)/(-4))-5</t>
-  </si>
-  <si>
-    <t>1-((-2))-5</t>
-  </si>
-  <si>
-    <t>((-2)/(-4))-5</t>
-  </si>
-  <si>
-    <t>((-2))-5</t>
-  </si>
-  <si>
-    <t>1-(-2-3)/(-4)-5</t>
-  </si>
-  <si>
-    <t>1+2+5</t>
-  </si>
-  <si>
-    <t>2/4+5</t>
-  </si>
-  <si>
-    <t>2+5</t>
-  </si>
-  <si>
-    <t>1+(2+3)/4+5</t>
-  </si>
-  <si>
-    <t>1+2/4+5</t>
-  </si>
-  <si>
-    <t>2+3+5</t>
-  </si>
-  <si>
-    <t>(2+3)/4+5</t>
-  </si>
-  <si>
-    <t>1+2+3+5</t>
-  </si>
-  <si>
     <t>pozitiven</t>
   </si>
   <si>
     <t>oklepaj zaradi</t>
   </si>
   <si>
-    <t>numer in denom</t>
-  </si>
-  <si>
-    <t>1-(-2)/(-4)-5</t>
-  </si>
-  <si>
     <t>http://tma.main.jp/logic/logic.php?lang=en&amp;type=4&amp;v0=a&amp;v1=b&amp;v2=c&amp;v3=d&amp;00=1&amp;01=1&amp;02=1&amp;03=0&amp;04=1&amp;05=1&amp;06=1&amp;07=0&amp;08=1&amp;09=0&amp;0a=1&amp;0b=0&amp;0c=0&amp;0d=0&amp;0e=0&amp;0f=0</t>
   </si>
   <si>
     <t>prvi v elementu</t>
+  </si>
+  <si>
+    <t>~a~c + ~a~d + ~b~d</t>
+  </si>
+  <si>
+    <t>numerator</t>
+  </si>
+  <si>
+    <t>denominator</t>
+  </si>
+  <si>
+    <t>1-((-2-3)/(-4-5))-6</t>
+  </si>
+  <si>
+    <t>1-((-2-3))-6</t>
+  </si>
+  <si>
+    <t>((-2-3)/(-4-5))-6</t>
+  </si>
+  <si>
+    <t>((-2-3))-6</t>
+  </si>
+  <si>
+    <t>1-((-2)/(-4))-6</t>
+  </si>
+  <si>
+    <t>1-((-2))-6</t>
+  </si>
+  <si>
+    <t>((-2)/(-4))-6</t>
+  </si>
+  <si>
+    <t>((-2))-6</t>
+  </si>
+  <si>
+    <t>1-(-2-3)/(-4-5)-6</t>
+  </si>
+  <si>
+    <t>1-(-2-3)-6</t>
+  </si>
+  <si>
+    <t>(-2-3)/(-4-5)-6</t>
+  </si>
+  <si>
+    <t>1-(-2)/(-4)-6</t>
+  </si>
+  <si>
+    <t>1-(-2)-6</t>
+  </si>
+  <si>
+    <t>1+(2+3)/(4+5)+6</t>
+  </si>
+  <si>
+    <t>1+2+3+6</t>
+  </si>
+  <si>
+    <t>(2+3)/(4+5)+6</t>
+  </si>
+  <si>
+    <t>2+3+6</t>
+  </si>
+  <si>
+    <t>1+2/4+6</t>
+  </si>
+  <si>
+    <t>1+2+6</t>
+  </si>
+  <si>
+    <t>2/4+6</t>
+  </si>
+  <si>
+    <t>2+6</t>
+  </si>
+  <si>
+    <t>1-((1)/(-4-5))-6</t>
+  </si>
+  <si>
+    <t>1-((1)/(-4))-6</t>
+  </si>
+  <si>
+    <t>1-1/(-4)-6</t>
+  </si>
+  <si>
+    <t>1+1/(4+5)+6</t>
+  </si>
+  <si>
+    <t>1/(4+5)+6</t>
+  </si>
+  <si>
+    <t>1+1/4+6</t>
+  </si>
+  <si>
+    <t>1/4+6</t>
+  </si>
+  <si>
+    <t>1-1/(-4-5)-6</t>
+  </si>
+  <si>
+    <t>http://tma.main.jp/logic/logic.php?lang=en&amp;type=3&amp;v0=a&amp;v1=b&amp;v2=c&amp;00=1&amp;01=1&amp;02=1&amp;03=1&amp;04=1&amp;05=1&amp;06=0&amp;07=0</t>
+  </si>
+  <si>
+    <t>~a + ~b</t>
+  </si>
+  <si>
+    <t>~a~d + ~b~d</t>
+  </si>
+  <si>
+    <t>imenovalec enočlenik</t>
   </si>
 </sst>
 </file>
@@ -172,10 +214,10 @@
   </cellStyleXfs>
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hiperpovezava" xfId="1" builtinId="8"/>
@@ -491,16 +533,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8DB5EFE3-4ACD-43EC-80C9-04FE5F9D8A36}">
-  <dimension ref="C5:J24"/>
+  <dimension ref="C3:J38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
-      <selection activeCell="I5" sqref="I5"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
+      <selection activeCell="I8" sqref="I8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="3" max="3" width="18" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.5703125" customWidth="1"/>
     <col min="5" max="5" width="14.5703125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="18" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="16" customWidth="1"/>
@@ -509,32 +551,51 @@
     <col min="10" max="10" width="17.28515625" customWidth="1"/>
   </cols>
   <sheetData>
+    <row r="3" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="G3" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="F4" t="s">
+        <v>7</v>
+      </c>
+      <c r="G4" t="s">
+        <v>6</v>
+      </c>
+    </row>
     <row r="5" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="G5" s="2" t="s">
-        <v>26</v>
+      <c r="F5" t="s">
+        <v>8</v>
+      </c>
+      <c r="G5" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="7" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="G7" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="H7" s="1"/>
+      <c r="G7" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="H7" s="2"/>
     </row>
     <row r="8" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C8" t="s">
-        <v>22</v>
+        <v>2</v>
       </c>
       <c r="D8" t="s">
         <v>1</v>
       </c>
       <c r="E8" t="s">
-        <v>27</v>
+        <v>5</v>
       </c>
       <c r="F8" t="s">
         <v>0</v>
       </c>
       <c r="G8" t="s">
-        <v>24</v>
+        <v>7</v>
+      </c>
+      <c r="H8" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="9" spans="3:10" x14ac:dyDescent="0.25">
@@ -553,11 +614,14 @@
       <c r="G9">
         <v>1</v>
       </c>
+      <c r="H9">
+        <v>1</v>
+      </c>
       <c r="I9" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="J9" t="s">
-        <v>3</v>
+        <v>9</v>
       </c>
     </row>
     <row r="10" spans="3:10" x14ac:dyDescent="0.25">
@@ -577,10 +641,10 @@
         <v>1</v>
       </c>
       <c r="I10" t="s">
-        <v>4</v>
+        <v>18</v>
       </c>
       <c r="J10" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
     </row>
     <row r="11" spans="3:10" x14ac:dyDescent="0.25">
@@ -599,11 +663,14 @@
       <c r="G11">
         <v>1</v>
       </c>
+      <c r="H11">
+        <v>1</v>
+      </c>
       <c r="I11" t="s">
-        <v>7</v>
+        <v>19</v>
       </c>
       <c r="J11" t="s">
-        <v>2</v>
+        <v>11</v>
       </c>
     </row>
     <row r="12" spans="3:10" x14ac:dyDescent="0.25">
@@ -620,11 +687,11 @@
         <v>1</v>
       </c>
       <c r="I12" t="str">
-        <f>"-2-3-5"</f>
-        <v>-2-3-5</v>
+        <f>"-2-3-6"</f>
+        <v>-2-3-6</v>
       </c>
       <c r="J12" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
     </row>
     <row r="13" spans="3:10" x14ac:dyDescent="0.25">
@@ -643,11 +710,14 @@
       <c r="G13">
         <v>1</v>
       </c>
+      <c r="H13">
+        <v>1</v>
+      </c>
       <c r="I13" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="J13" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
     </row>
     <row r="14" spans="3:10" x14ac:dyDescent="0.25">
@@ -667,10 +737,10 @@
         <v>1</v>
       </c>
       <c r="I14" t="s">
-        <v>6</v>
+        <v>21</v>
       </c>
       <c r="J14" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
     </row>
     <row r="15" spans="3:10" x14ac:dyDescent="0.25">
@@ -689,12 +759,15 @@
       <c r="G15">
         <v>1</v>
       </c>
+      <c r="H15">
+        <v>1</v>
+      </c>
       <c r="I15" t="str">
-        <f>"-2/(-4)-5"</f>
-        <v>-2/(-4)-5</v>
+        <f>"-2/(-4)-6"</f>
+        <v>-2/(-4)-6</v>
       </c>
       <c r="J15" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
     </row>
     <row r="16" spans="3:10" x14ac:dyDescent="0.25">
@@ -711,11 +784,11 @@
         <v>1</v>
       </c>
       <c r="I16" t="str">
-        <f>"-2-5"</f>
-        <v>-2-5</v>
+        <f>"-2-6"</f>
+        <v>-2-6</v>
       </c>
       <c r="J16" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
     </row>
     <row r="17" spans="3:9" x14ac:dyDescent="0.25">
@@ -734,8 +807,11 @@
       <c r="G17">
         <v>1</v>
       </c>
+      <c r="H17">
+        <v>1</v>
+      </c>
       <c r="I17" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
     </row>
     <row r="18" spans="3:9" x14ac:dyDescent="0.25">
@@ -752,7 +828,7 @@
         <v>1</v>
       </c>
       <c r="I18" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="19" spans="3:9" x14ac:dyDescent="0.25">
@@ -771,8 +847,11 @@
       <c r="G19">
         <v>1</v>
       </c>
+      <c r="H19">
+        <v>1</v>
+      </c>
       <c r="I19" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
     </row>
     <row r="20" spans="3:9" x14ac:dyDescent="0.25">
@@ -789,7 +868,7 @@
         <v>1</v>
       </c>
       <c r="I20" t="s">
-        <v>19</v>
+        <v>25</v>
       </c>
     </row>
     <row r="21" spans="3:9" x14ac:dyDescent="0.25">
@@ -806,7 +885,7 @@
         <v>0</v>
       </c>
       <c r="I21" t="s">
-        <v>18</v>
+        <v>26</v>
       </c>
     </row>
     <row r="22" spans="3:9" x14ac:dyDescent="0.25">
@@ -823,7 +902,7 @@
         <v>1</v>
       </c>
       <c r="I22" t="s">
-        <v>14</v>
+        <v>27</v>
       </c>
     </row>
     <row r="23" spans="3:9" x14ac:dyDescent="0.25">
@@ -840,7 +919,7 @@
         <v>0</v>
       </c>
       <c r="I23" t="s">
-        <v>15</v>
+        <v>28</v>
       </c>
     </row>
     <row r="24" spans="3:9" x14ac:dyDescent="0.25">
@@ -857,7 +936,177 @@
         <v>1</v>
       </c>
       <c r="I24" t="s">
-        <v>16</v>
+        <v>29</v>
+      </c>
+    </row>
+    <row r="27" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="E27" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="28" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="E28" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="30" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C30" t="s">
+        <v>2</v>
+      </c>
+      <c r="D30" t="s">
+        <v>41</v>
+      </c>
+      <c r="E30" t="s">
+        <v>5</v>
+      </c>
+      <c r="F30" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="31" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C31">
+        <v>0</v>
+      </c>
+      <c r="D31">
+        <v>0</v>
+      </c>
+      <c r="E31">
+        <v>0</v>
+      </c>
+      <c r="F31">
+        <v>1</v>
+      </c>
+      <c r="G31" t="s">
+        <v>37</v>
+      </c>
+      <c r="H31" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="32" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C32">
+        <v>0</v>
+      </c>
+      <c r="D32">
+        <v>0</v>
+      </c>
+      <c r="E32">
+        <v>1</v>
+      </c>
+      <c r="F32">
+        <v>1</v>
+      </c>
+      <c r="G32" t="str">
+        <f>"-1/(-4-5)-6"</f>
+        <v>-1/(-4-5)-6</v>
+      </c>
+      <c r="H32" t="str">
+        <f>"-((1)/(-4-5))-6"</f>
+        <v>-((1)/(-4-5))-6</v>
+      </c>
+    </row>
+    <row r="33" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C33">
+        <v>0</v>
+      </c>
+      <c r="D33">
+        <v>1</v>
+      </c>
+      <c r="E33">
+        <v>0</v>
+      </c>
+      <c r="F33">
+        <v>1</v>
+      </c>
+      <c r="G33" t="s">
+        <v>32</v>
+      </c>
+      <c r="H33" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="34" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C34">
+        <v>0</v>
+      </c>
+      <c r="D34">
+        <v>1</v>
+      </c>
+      <c r="E34">
+        <v>1</v>
+      </c>
+      <c r="F34">
+        <v>1</v>
+      </c>
+      <c r="G34" t="str">
+        <f>"-1/(-4)-6"</f>
+        <v>-1/(-4)-6</v>
+      </c>
+      <c r="H34" t="str">
+        <f>"-((1)/(-4))-6"</f>
+        <v>-((1)/(-4))-6</v>
+      </c>
+    </row>
+    <row r="35" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C35">
+        <v>1</v>
+      </c>
+      <c r="D35">
+        <v>0</v>
+      </c>
+      <c r="E35">
+        <v>0</v>
+      </c>
+      <c r="F35">
+        <v>1</v>
+      </c>
+      <c r="G35" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="36" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C36">
+        <v>1</v>
+      </c>
+      <c r="D36">
+        <v>0</v>
+      </c>
+      <c r="E36">
+        <v>1</v>
+      </c>
+      <c r="F36">
+        <v>1</v>
+      </c>
+      <c r="G36" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="37" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C37">
+        <v>1</v>
+      </c>
+      <c r="D37">
+        <v>1</v>
+      </c>
+      <c r="E37">
+        <v>0</v>
+      </c>
+      <c r="G37" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="38" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C38">
+        <v>1</v>
+      </c>
+      <c r="D38">
+        <v>1</v>
+      </c>
+      <c r="E38">
+        <v>1</v>
+      </c>
+      <c r="G38" t="s">
+        <v>36</v>
       </c>
     </row>
   </sheetData>
@@ -866,7 +1115,7 @@
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="G5" r:id="rId1" xr:uid="{BE4F2CDD-D7E1-408D-B874-BA2940A85FB4}"/>
+    <hyperlink ref="G3" r:id="rId1" xr:uid="{BE4F2CDD-D7E1-408D-B874-BA2940A85FB4}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
idea for to string in formulas
</commit_message>
<xml_diff>
--- a/truth table.xlsx
+++ b/truth table.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\dev\rust\math-eval\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D29447D-351D-4E1C-943B-2DC61A2F8B08}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5249AE1E-1E76-4513-942D-985F4CFB8D2E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1035" yWindow="1050" windowWidth="38700" windowHeight="15885" activeTab="1" xr2:uid="{D11C0042-871A-40E6-9C8F-06A0F0CE9C5E}"/>
+    <workbookView xWindow="-105" yWindow="0" windowWidth="26010" windowHeight="21705" activeTab="1" xr2:uid="{D11C0042-871A-40E6-9C8F-06A0F0CE9C5E}"/>
   </bookViews>
   <sheets>
     <sheet name="List1" sheetId="1" r:id="rId1"/>
     <sheet name="List2" sheetId="2" r:id="rId2"/>
+    <sheet name="List3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="45">
   <si>
     <t>prazen imenovalec</t>
   </si>
@@ -169,6 +170,9 @@
   </si>
   <si>
     <t>~b~d + ~a</t>
+  </si>
+  <si>
+    <t>1-(((-2-3)*(-4-5))/((-6-7)*(-8-9)))</t>
   </si>
 </sst>
 </file>
@@ -532,7 +536,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme 2013 - 2022" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -542,7 +546,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8DB5EFE3-4ACD-43EC-80C9-04FE5F9D8A36}">
   <dimension ref="C3:M38"/>
   <sheetViews>
-    <sheetView topLeftCell="A22" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
+    <sheetView topLeftCell="F1" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
       <selection activeCell="C30" sqref="C30:H38"/>
     </sheetView>
   </sheetViews>
@@ -1159,7 +1163,7 @@
   <dimension ref="E6:M34"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="G1" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
-      <selection activeCell="L8" sqref="L8:L23"/>
+      <selection activeCell="M8" sqref="M8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1715,4 +1719,27 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D5E981DE-46EA-495E-91FA-884FEE494070}">
+  <dimension ref="E8"/>
+  <sheetViews>
+    <sheetView zoomScale="265" zoomScaleNormal="265" workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="5" max="5" width="32.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="8" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E8" t="s">
+        <v>44</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>